<commit_message>
feat: añado los datos de copkmeans originales
</commit_message>
<xml_diff>
--- a/analisis/Segunda Memoria/Tablas_PAR_2020-21.xlsx
+++ b/analisis/Segunda Memoria/Tablas_PAR_2020-21.xlsx
@@ -212,7 +212,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <name val="Arial"/>
       <color theme="1"/>
@@ -258,6 +258,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <color rgb="FF9C6500"/>
+      <sz val="11.000000"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <name val="Times New Roman"/>
       <b/>
       <sz val="12.000000"/>
@@ -296,7 +302,7 @@
       <sz val="12.000000"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -332,6 +338,12 @@
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor theme="6" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -607,7 +619,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="14">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -621,95 +633,96 @@
     <xf fontId="5" fillId="5" borderId="3" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1"/>
     <xf fontId="6" fillId="6" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="2" fillId="7" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
+    <xf fontId="7" fillId="8" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
   <cellXfs count="37">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="7" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="8" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="7" fillId="0" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="8" fillId="0" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="8" fillId="0" borderId="6" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf fontId="9" fillId="0" borderId="6" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf fontId="7" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="10" fillId="0" borderId="6" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf fontId="8" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="10" fillId="6" borderId="0" numFmtId="0" xfId="12" applyFont="1" applyFill="1"/>
-    <xf fontId="11" fillId="3" borderId="0" numFmtId="0" xfId="7" applyFont="1" applyFill="1"/>
+    <xf fontId="11" fillId="6" borderId="0" numFmtId="0" xfId="12" applyFont="1" applyFill="1"/>
+    <xf fontId="12" fillId="3" borderId="0" numFmtId="0" xfId="7" applyFont="1" applyFill="1"/>
     <xf fontId="3" fillId="4" borderId="1" numFmtId="0" xfId="8" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="7" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="10" fillId="6" borderId="0" numFmtId="0" xfId="11" applyFont="1" applyFill="1"/>
+    <xf fontId="11" fillId="6" borderId="0" numFmtId="0" xfId="11" applyFont="1" applyFill="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="12" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="13" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="12" fillId="0" borderId="8" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="13" fillId="0" borderId="8" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="7" fillId="0" borderId="4" numFmtId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="8" fillId="0" borderId="4" numFmtId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="7" fillId="0" borderId="9" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="8" fillId="0" borderId="9" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="7" fillId="0" borderId="10" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="8" fillId="0" borderId="10" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="13" fillId="0" borderId="11" numFmtId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="14" fillId="0" borderId="11" numFmtId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="14" fillId="0" borderId="12" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="14" fillId="0" borderId="11" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="8" fillId="0" borderId="13" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="8" fillId="0" borderId="14" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="8" fillId="0" borderId="11" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="15" numFmtId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="15" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="13" fillId="0" borderId="15" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="13" fillId="0" borderId="16" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="8" fillId="0" borderId="17" numFmtId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="8" fillId="0" borderId="18" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="8" fillId="0" borderId="19" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="8" fillId="0" borderId="12" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="13" fillId="0" borderId="12" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="13" fillId="0" borderId="11" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="8" fillId="0" borderId="17" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="7" fillId="0" borderId="13" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="8" fillId="0" borderId="20" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="7" fillId="0" borderId="14" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="7" fillId="0" borderId="11" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="15" numFmtId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="15" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="12" fillId="0" borderId="15" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="12" fillId="0" borderId="16" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="7" fillId="0" borderId="17" numFmtId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="7" fillId="0" borderId="18" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="7" fillId="0" borderId="19" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="7" fillId="0" borderId="12" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="12" fillId="0" borderId="12" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="7" fillId="0" borderId="17" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="7" fillId="0" borderId="20" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="7" fillId="0" borderId="21" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="7" fillId="8" borderId="0" numFmtId="0" xfId="13" applyFont="1" applyFill="1"/>
+    <xf fontId="8" fillId="0" borderId="21" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="14">
     <cellStyle name="Style 1" xfId="0" builtinId="0"/>
     <cellStyle name="Style 2" xfId="1" builtinId="3"/>
     <cellStyle name="Style 3" xfId="2" builtinId="6"/>
@@ -723,6 +736,7 @@
     <cellStyle name="Heading 3" xfId="10" builtinId="18"/>
     <cellStyle name="60% - Accent1" xfId="11" builtinId="32"/>
     <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="Neutral" xfId="13" builtinId="28"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1157,12 +1171,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" customHeight="1" defaultRowHeight="13"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="24.421875"/>
-    <col customWidth="1" min="2" max="2" width="32.28125"/>
+    <col bestFit="1" customWidth="1" min="1" max="1" width="24.421875"/>
+    <col bestFit="1" customWidth="1" min="2" max="2" width="32.28125"/>
     <col bestFit="1" customWidth="1" min="3" max="4" width="11.019500000000001"/>
-    <col customWidth="1" min="5" max="5" width="21.7109375"/>
-    <col customWidth="1" min="6" max="6" width="18.8515625"/>
-    <col customWidth="1" min="7" max="7" width="22.140625"/>
+    <col bestFit="1" customWidth="1" min="5" max="5" width="21.7109375"/>
+    <col bestFit="1" customWidth="1" min="6" max="6" width="18.8515625"/>
+    <col bestFit="1" customWidth="1" min="7" max="7" width="22.140625"/>
     <col bestFit="1" customWidth="1" min="8" max="8" width="11.019500000000001"/>
     <col bestFit="1" customWidth="1" min="9" max="9" width="17.074200000000001"/>
     <col bestFit="1" customWidth="1" min="10" max="257" width="11.019500000000001"/>
@@ -1316,7 +1330,7 @@
       <c r="G10" s="6"/>
       <c r="O10" s="6"/>
     </row>
-    <row r="11" ht="30">
+    <row r="11" ht="14.25">
       <c r="A11" s="7" t="s">
         <v>12</v>
       </c>
@@ -1460,7 +1474,7 @@
       </c>
       <c r="O16" s="5"/>
     </row>
-    <row r="17" ht="30">
+    <row r="17" ht="14.25">
       <c r="A17" s="8" t="s">
         <v>21</v>
       </c>
@@ -2227,7 +2241,7 @@
       <c r="G51" s="6"/>
     </row>
     <row r="52" ht="13" customHeight="1">
-      <c r="A52" s="11" t="s">
+      <c r="A52" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B52" s="6"/>
@@ -8232,7 +8246,7 @@
       <c r="T315" s="6"/>
     </row>
     <row r="316" ht="13" customHeight="1">
-      <c r="A316" s="11" t="s">
+      <c r="A316" s="6" t="s">
         <v>47</v>
       </c>
       <c r="B316" s="6"/>
@@ -8256,25 +8270,25 @@
       <c r="T316" s="6"/>
     </row>
     <row r="317" ht="13" customHeight="1">
-      <c r="A317" s="12" t="s">
+      <c r="A317" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B317" s="12" t="s">
+      <c r="B317" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C317" s="12" t="s">
+      <c r="C317" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D317" s="12" t="s">
+      <c r="D317" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E317" s="12" t="s">
+      <c r="E317" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F317" s="12" t="s">
+      <c r="F317" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G317" s="12" t="s">
+      <c r="G317" s="11" t="s">
         <v>18</v>
       </c>
       <c r="H317" s="6"/>
@@ -8821,81 +8835,81 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="48.00390625"/>
-    <col customWidth="1" min="2" max="2" style="13" width="17.140625"/>
+    <col bestFit="1" customWidth="1" min="1" max="1" width="48.00390625"/>
+    <col bestFit="1" customWidth="1" min="2" max="2" style="12" width="17.140625"/>
     <col bestFit="1" customWidth="1" min="3" max="3" width="18.00390625"/>
     <col bestFit="1" min="4" max="4" width="7.28125"/>
-    <col customWidth="1" min="5" max="5" width="15.421875"/>
+    <col bestFit="1" customWidth="1" min="5" max="5" width="15.421875"/>
     <col bestFit="1" min="6" max="6" width="12.00390625"/>
-    <col customWidth="1" min="7" max="7" width="23.140625"/>
-    <col customWidth="1" min="8" max="8" width="20.140625"/>
+    <col bestFit="1" customWidth="1" min="7" max="7" width="23.140625"/>
+    <col bestFit="1" customWidth="1" min="8" max="8" width="20.140625"/>
     <col bestFit="1" min="9" max="9" width="4.7109375"/>
     <col bestFit="1" min="10" max="10" width="12.00390625"/>
-    <col customWidth="1" min="11" max="11" width="20.28125"/>
+    <col bestFit="1" customWidth="1" min="11" max="11" width="20.28125"/>
     <col bestFit="1" min="12" max="12" width="7.28125"/>
-    <col customWidth="1" min="13" max="13" width="20.421875"/>
+    <col bestFit="1" customWidth="1" min="13" max="13" width="20.421875"/>
   </cols>
   <sheetData>
     <row r="1" ht="15">
-      <c r="B1" s="13"/>
-      <c r="G1" s="14" t="s">
+      <c r="B1" s="12"/>
+      <c r="G1" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="2" ht="12.75">
-      <c r="A2" s="15"/>
-      <c r="B2" s="16" t="s">
+      <c r="A2" s="14"/>
+      <c r="B2" s="15" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="18" t="s">
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
     </row>
     <row r="3" ht="15">
-      <c r="A3" s="15"/>
-      <c r="B3" s="19" t="s">
+      <c r="A3" s="14"/>
+      <c r="B3" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="20" t="s">
         <v>52</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="20" t="s">
         <v>52</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="J3" s="21" t="s">
+      <c r="J3" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="K3" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="L3" s="21" t="s">
+      <c r="L3" s="20" t="s">
         <v>52</v>
       </c>
       <c r="M3" s="2" t="s">
@@ -8903,12 +8917,48 @@
       </c>
     </row>
     <row r="4" ht="15">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="21" t="s">
         <v>54</v>
       </c>
+      <c r="B4" s="12">
+        <v>21.600000000000001</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0.089999999999999997</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0.22</v>
+      </c>
+      <c r="F4" s="6">
+        <v>16</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="H4" s="6">
+        <v>0.39000000000000001</v>
+      </c>
+      <c r="I4" s="6">
+        <v>0.93000000000000005</v>
+      </c>
+      <c r="J4" s="6">
+        <v>79.200000000000003</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="L4" s="6">
+        <v>0.26000000000000001</v>
+      </c>
+      <c r="M4" s="6">
+        <v>6.8399999999999999</v>
+      </c>
     </row>
     <row r="5" ht="19.5" customHeight="1">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="22" t="s">
         <v>55</v>
       </c>
       <c r="B5">
@@ -8949,7 +8999,7 @@
       </c>
     </row>
     <row r="6" ht="19.5" customHeight="1">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="23" t="s">
         <v>56</v>
       </c>
       <c r="B6">
@@ -8990,7 +9040,7 @@
       </c>
     </row>
     <row r="7" ht="19.5" customHeight="1">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="23" t="s">
         <v>57</v>
       </c>
       <c r="B7">
@@ -9031,7 +9081,7 @@
       </c>
     </row>
     <row r="8" ht="19.5" customHeight="1">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="23" t="s">
         <v>58</v>
       </c>
       <c r="B8">
@@ -9072,7 +9122,7 @@
       </c>
     </row>
     <row r="9" ht="19.5" customHeight="1">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="23" t="s">
         <v>59</v>
       </c>
       <c r="B9">
@@ -9113,7 +9163,7 @@
       </c>
     </row>
     <row r="10" ht="19.5" customHeight="1">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="23" t="s">
         <v>60</v>
       </c>
       <c r="B10">
@@ -9154,7 +9204,7 @@
       </c>
     </row>
     <row r="11" ht="19.5" customHeight="1">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="23" t="s">
         <v>61</v>
       </c>
       <c r="B11">
@@ -9195,7 +9245,7 @@
       </c>
     </row>
     <row r="12" ht="19.5" customHeight="1">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="23" t="s">
         <v>62</v>
       </c>
       <c r="B12">
@@ -9238,75 +9288,75 @@
     <row r="13" ht="19.5" customHeight="1"/>
     <row r="14" ht="19.5" customHeight="1">
       <c r="A14" s="6"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="27" t="s">
+      <c r="B14" s="24"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="26"/>
-      <c r="M14" s="26"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="25"/>
+      <c r="M14" s="25"/>
     </row>
     <row r="15" ht="19.5" customHeight="1">
-      <c r="A15" s="28"/>
-      <c r="B15" s="29" t="s">
+      <c r="A15" s="27"/>
+      <c r="B15" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="31" t="s">
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="31" t="s">
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="32"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="31"/>
     </row>
     <row r="16" ht="19.5" customHeight="1">
-      <c r="A16" s="33"/>
-      <c r="B16" s="19" t="s">
+      <c r="A16" s="32"/>
+      <c r="B16" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="21" t="s">
+      <c r="D16" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="E16" s="34" t="s">
+      <c r="E16" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="F16" s="21" t="s">
+      <c r="F16" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="G16" s="21" t="s">
+      <c r="G16" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="H16" s="21" t="s">
+      <c r="H16" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="I16" s="34" t="s">
+      <c r="I16" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="J16" s="21" t="s">
+      <c r="J16" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="K16" s="21" t="s">
+      <c r="K16" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="L16" s="21" t="s">
+      <c r="L16" s="20" t="s">
         <v>52</v>
       </c>
       <c r="M16" s="2" t="s">
@@ -9314,8 +9364,44 @@
       </c>
     </row>
     <row r="17" ht="19.5" customHeight="1">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="34" t="s">
         <v>54</v>
+      </c>
+      <c r="B17" s="12">
+        <v>7.4000000000000004</v>
+      </c>
+      <c r="C17">
+        <v>0.089999999999999997</v>
+      </c>
+      <c r="D17">
+        <v>1.03</v>
+      </c>
+      <c r="E17">
+        <v>0.22</v>
+      </c>
+      <c r="F17">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="G17">
+        <v>-0.01</v>
+      </c>
+      <c r="H17">
+        <v>0.34999999999999998</v>
+      </c>
+      <c r="I17">
+        <v>0.34999999999999998</v>
+      </c>
+      <c r="J17" s="35">
+        <v>0</v>
+      </c>
+      <c r="K17" s="35">
+        <v>0</v>
+      </c>
+      <c r="L17" s="35">
+        <v>0</v>
+      </c>
+      <c r="M17" s="35">
+        <v>0</v>
       </c>
     </row>
     <row r="18" ht="19.5" customHeight="1">
@@ -9360,7 +9446,7 @@
       </c>
     </row>
     <row r="19" ht="19.5" customHeight="1">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="23" t="s">
         <v>56</v>
       </c>
       <c r="B19">
@@ -9401,7 +9487,7 @@
       </c>
     </row>
     <row r="20" ht="19.5" customHeight="1">
-      <c r="A20" s="24" t="s">
+      <c r="A20" s="23" t="s">
         <v>57</v>
       </c>
       <c r="B20">
@@ -9442,7 +9528,7 @@
       </c>
     </row>
     <row r="21" ht="19.5" customHeight="1">
-      <c r="A21" s="24" t="s">
+      <c r="A21" s="23" t="s">
         <v>58</v>
       </c>
       <c r="B21">
@@ -9483,7 +9569,7 @@
       </c>
     </row>
     <row r="22" ht="19.5" customHeight="1">
-      <c r="A22" s="24" t="s">
+      <c r="A22" s="23" t="s">
         <v>59</v>
       </c>
       <c r="B22">
@@ -9524,7 +9610,7 @@
       </c>
     </row>
     <row r="23" ht="19.5" customHeight="1">
-      <c r="A23" s="24" t="s">
+      <c r="A23" s="23" t="s">
         <v>60</v>
       </c>
       <c r="B23">
@@ -9565,7 +9651,7 @@
       </c>
     </row>
     <row r="24" ht="19.5" customHeight="1">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="23" t="s">
         <v>61</v>
       </c>
       <c r="B24">
@@ -9606,7 +9692,7 @@
       </c>
     </row>
     <row r="25" ht="19.5" customHeight="1">
-      <c r="A25" s="24" t="s">
+      <c r="A25" s="23" t="s">
         <v>62</v>
       </c>
       <c r="B25">

</xml_diff>

<commit_message>
fix: solucionamos el problema con el memetico elitista
</commit_message>
<xml_diff>
--- a/analisis/Segunda Memoria/Tablas_PAR_2020-21.xlsx
+++ b/analisis/Segunda Memoria/Tablas_PAR_2020-21.xlsx
@@ -635,7 +635,7 @@
     <xf fontId="2" fillId="7" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="7" fillId="8" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="8" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -717,7 +717,6 @@
     <xf fontId="8" fillId="0" borderId="20" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="7" fillId="8" borderId="0" numFmtId="0" xfId="13" applyFont="1" applyFill="1"/>
     <xf fontId="8" fillId="0" borderId="21" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -9391,21 +9390,21 @@
       <c r="I17">
         <v>0.34999999999999998</v>
       </c>
-      <c r="J17" s="35">
-        <v>0</v>
-      </c>
-      <c r="K17" s="35">
-        <v>0</v>
-      </c>
-      <c r="L17" s="35">
-        <v>0</v>
-      </c>
-      <c r="M17" s="35">
-        <v>0</v>
+      <c r="J17" s="6">
+        <v>2163</v>
+      </c>
+      <c r="K17" s="6">
+        <v>0.25536830945193267</v>
+      </c>
+      <c r="L17" s="6">
+        <v>0.55697927079143317</v>
+      </c>
+      <c r="M17" s="6">
+        <v>0.0037180750000000004</v>
       </c>
     </row>
     <row r="18" ht="19.5" customHeight="1">
-      <c r="A18" s="36" t="s">
+      <c r="A18" s="35" t="s">
         <v>55</v>
       </c>
       <c r="B18">

</xml_diff>

<commit_message>
feat: tabla de datos actualizada
</commit_message>
<xml_diff>
--- a/analisis/Segunda Memoria/Tablas_PAR_2020-21.xlsx
+++ b/analisis/Segunda Memoria/Tablas_PAR_2020-21.xlsx
@@ -212,7 +212,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <name val="Arial"/>
       <color theme="1"/>
@@ -300,6 +300,12 @@
       <b/>
       <i/>
       <sz val="12.000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color rgb="FF006100"/>
+      <sz val="10.000000"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -635,7 +641,7 @@
     <xf fontId="2" fillId="7" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="7" fillId="8" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="8" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -688,6 +694,7 @@
     <xf fontId="8" fillId="0" borderId="11" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf fontId="15" fillId="2" borderId="0" numFmtId="0" xfId="6" applyFont="1" applyFill="1"/>
     <xf fontId="0" fillId="0" borderId="15" numFmtId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="15" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="13" fillId="0" borderId="15" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -8828,7 +8835,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100">
+    <sheetView showGridLines="1" showRowColHeaders="1" workbookViewId="0" zoomScale="100">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -8966,7 +8973,7 @@
       <c r="C5">
         <v>0.68008493299999995</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="6">
         <v>0.75586127000000003</v>
       </c>
       <c r="E5">
@@ -9007,7 +9014,7 @@
       <c r="C6">
         <v>0.62335108100000003</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="6">
         <v>0.66427030300000001</v>
       </c>
       <c r="E6">
@@ -9048,7 +9055,7 @@
       <c r="C7">
         <v>0.60010004400000005</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="6">
         <v>0.64101926600000003</v>
       </c>
       <c r="E7">
@@ -9089,7 +9096,7 @@
       <c r="C8">
         <v>0.69585739300000005</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="6">
         <v>0.74321760400000003</v>
       </c>
       <c r="E8">
@@ -9130,7 +9137,7 @@
       <c r="C9">
         <v>0.65188900900000002</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="6">
         <v>0.700385865</v>
       </c>
       <c r="E9">
@@ -9171,7 +9178,7 @@
       <c r="C10">
         <v>0.691463508</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="6">
         <v>0.75511563000000004</v>
       </c>
       <c r="E10">
@@ -9212,7 +9219,7 @@
       <c r="C11">
         <v>0.62873728600000001</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="6">
         <v>0.70148257000000003</v>
       </c>
       <c r="E11">
@@ -9248,83 +9255,83 @@
         <v>62</v>
       </c>
       <c r="B12">
-        <v>10</v>
-      </c>
-      <c r="C12">
-        <v>0.68733788200000001</v>
-      </c>
-      <c r="D12">
-        <v>0.76311421899999998</v>
-      </c>
-      <c r="E12">
-        <v>1.361656647</v>
-      </c>
-      <c r="F12">
-        <v>154.40000000000001</v>
-      </c>
-      <c r="G12">
-        <v>0.26685197199999999</v>
-      </c>
-      <c r="H12">
-        <v>0.41878789199999999</v>
-      </c>
-      <c r="I12">
-        <v>3.253448771</v>
-      </c>
-      <c r="J12">
-        <v>884.79999999999995</v>
-      </c>
-      <c r="K12">
-        <v>0.23090981399999999</v>
-      </c>
-      <c r="L12">
-        <v>0.46802580999999999</v>
-      </c>
-      <c r="M12">
-        <v>6.7316101980000003</v>
+        <v>7</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0.59048100820771687</v>
+      </c>
+      <c r="D12" s="24">
+        <v>0.64352444392715802</v>
+      </c>
+      <c r="E12" s="6">
+        <v>1.3895912319999999</v>
+      </c>
+      <c r="F12" s="6">
+        <v>39</v>
+      </c>
+      <c r="G12" s="6">
+        <v>0.19352668288310054</v>
+      </c>
+      <c r="H12" s="6">
+        <v>0.23190427931161395</v>
+      </c>
+      <c r="I12" s="6">
+        <v>3.2998014150000001</v>
+      </c>
+      <c r="J12" s="6">
+        <v>230</v>
+      </c>
+      <c r="K12" s="6">
+        <v>0.14082618310918626</v>
+      </c>
+      <c r="L12" s="6">
+        <v>0.20246347864991721</v>
+      </c>
+      <c r="M12" s="6">
+        <v>6.718178838</v>
       </c>
     </row>
     <row r="13" ht="19.5" customHeight="1"/>
     <row r="14" ht="19.5" customHeight="1">
       <c r="A14" s="6"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="26" t="s">
+      <c r="B14" s="25"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="25"/>
-      <c r="L14" s="25"/>
-      <c r="M14" s="25"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="26"/>
     </row>
     <row r="15" ht="19.5" customHeight="1">
-      <c r="A15" s="27"/>
-      <c r="B15" s="28" t="s">
+      <c r="A15" s="28"/>
+      <c r="B15" s="29" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="30" t="s">
+      <c r="E15" s="30"/>
+      <c r="F15" s="31" t="s">
         <v>9</v>
       </c>
       <c r="G15" s="16"/>
       <c r="H15" s="16"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="30" t="s">
+      <c r="I15" s="30"/>
+      <c r="J15" s="31" t="s">
         <v>10</v>
       </c>
       <c r="K15" s="16"/>
       <c r="L15" s="16"/>
-      <c r="M15" s="31"/>
+      <c r="M15" s="32"/>
     </row>
     <row r="16" ht="19.5" customHeight="1">
-      <c r="A16" s="32"/>
+      <c r="A16" s="33"/>
       <c r="B16" s="18" t="s">
         <v>50</v>
       </c>
@@ -9334,7 +9341,7 @@
       <c r="D16" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="E16" s="33" t="s">
+      <c r="E16" s="34" t="s">
         <v>53</v>
       </c>
       <c r="F16" s="20" t="s">
@@ -9346,7 +9353,7 @@
       <c r="H16" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="I16" s="33" t="s">
+      <c r="I16" s="34" t="s">
         <v>53</v>
       </c>
       <c r="J16" s="20" t="s">
@@ -9363,7 +9370,7 @@
       </c>
     </row>
     <row r="17" ht="19.5" customHeight="1">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="35" t="s">
         <v>54</v>
       </c>
       <c r="B17" s="12">
@@ -9404,7 +9411,7 @@
       </c>
     </row>
     <row r="18" ht="19.5" customHeight="1">
-      <c r="A18" s="35" t="s">
+      <c r="A18" s="36" t="s">
         <v>55</v>
       </c>
       <c r="B18">
@@ -9695,40 +9702,40 @@
         <v>62</v>
       </c>
       <c r="B25">
-        <v>10.800000000000001</v>
-      </c>
-      <c r="C25">
-        <v>0.73063136399999995</v>
-      </c>
-      <c r="D25">
-        <v>0.77424263999999998</v>
-      </c>
-      <c r="E25">
-        <v>1.591715102</v>
+        <v>29</v>
+      </c>
+      <c r="C25" s="6">
+        <v>0.60394656653534784</v>
+      </c>
+      <c r="D25" s="6">
+        <v>0.72105091851370062</v>
+      </c>
+      <c r="E25" s="6">
+        <v>1.6418014740000002</v>
       </c>
       <c r="F25">
-        <v>22.5</v>
-      </c>
-      <c r="G25">
-        <v>0.25988999899999998</v>
-      </c>
-      <c r="H25">
-        <v>0.37702714700000001</v>
-      </c>
-      <c r="I25">
-        <v>4.3487923610000001</v>
+        <v>29</v>
+      </c>
+      <c r="G25" s="6">
+        <v>0.25109115900159085</v>
+      </c>
+      <c r="H25" s="6">
+        <v>0.26236741667298302</v>
+      </c>
+      <c r="I25" s="6">
+        <v>4.4297566579999996</v>
       </c>
       <c r="J25">
-        <v>1650.5999999999999</v>
-      </c>
-      <c r="K25">
-        <v>0.213226954</v>
-      </c>
-      <c r="L25">
-        <v>0.44338832900000003</v>
-      </c>
-      <c r="M25">
-        <v>9.6424067339999997</v>
+        <v>488</v>
+      </c>
+      <c r="K25" s="6">
+        <v>0.12794817952009666</v>
+      </c>
+      <c r="L25" s="6">
+        <v>0.19932011084591655</v>
+      </c>
+      <c r="M25" s="6">
+        <v>9.7775687439999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: seguimos trabajando en la memoria, con los analisis
</commit_message>
<xml_diff>
--- a/analisis/Segunda Memoria/Tablas_PAR_2020-21.xlsx
+++ b/analisis/Segunda Memoria/Tablas_PAR_2020-21.xlsx
@@ -264,6 +264,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <color rgb="FF9C0006"/>
+      <sz val="11.000000"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <name val="Times New Roman"/>
       <b/>
       <sz val="12.000000"/>
@@ -301,14 +307,8 @@
       <i/>
       <sz val="12.000000"/>
     </font>
-    <font>
-      <name val="Calibri"/>
-      <color rgb="FF006100"/>
-      <sz val="10.000000"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -350,6 +350,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -625,7 +631,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="14">
+  <cellStyleXfs count="15">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -640,95 +646,97 @@
     <xf fontId="6" fillId="6" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="2" fillId="7" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="7" fillId="8" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
+    <xf fontId="8" fillId="9" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="8" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="9" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="8" fillId="0" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="9" fillId="0" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="9" fillId="0" borderId="6" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf fontId="10" fillId="0" borderId="6" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf fontId="8" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="11" fillId="0" borderId="6" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf fontId="9" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="11" fillId="6" borderId="0" numFmtId="0" xfId="12" applyFont="1" applyFill="1"/>
-    <xf fontId="12" fillId="3" borderId="0" numFmtId="0" xfId="7" applyFont="1" applyFill="1"/>
+    <xf fontId="12" fillId="6" borderId="0" numFmtId="0" xfId="12" applyFont="1" applyFill="1"/>
+    <xf fontId="13" fillId="3" borderId="0" numFmtId="0" xfId="7" applyFont="1" applyFill="1"/>
     <xf fontId="3" fillId="4" borderId="1" numFmtId="0" xfId="8" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="7" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="11" fillId="6" borderId="0" numFmtId="0" xfId="11" applyFont="1" applyFill="1"/>
+    <xf fontId="12" fillId="6" borderId="0" numFmtId="0" xfId="11" applyFont="1" applyFill="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="13" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="14" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="13" fillId="0" borderId="8" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="14" fillId="0" borderId="8" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="8" fillId="0" borderId="4" numFmtId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="9" fillId="0" borderId="4" numFmtId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="8" fillId="0" borderId="9" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="9" fillId="0" borderId="9" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="8" fillId="0" borderId="10" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="9" fillId="0" borderId="10" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="14" fillId="0" borderId="11" numFmtId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="15" fillId="0" borderId="11" numFmtId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="15" fillId="0" borderId="12" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="15" fillId="0" borderId="11" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="9" fillId="0" borderId="13" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="8" fillId="9" borderId="0" numFmtId="0" xfId="14" applyFont="1" applyFill="1"/>
+    <xf fontId="9" fillId="0" borderId="14" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="6" applyFont="1" applyFill="1"/>
+    <xf fontId="9" fillId="0" borderId="11" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="15" numFmtId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="15" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="14" fillId="0" borderId="15" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="14" fillId="0" borderId="16" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="9" fillId="0" borderId="17" numFmtId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="9" fillId="0" borderId="18" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="9" fillId="0" borderId="19" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="9" fillId="0" borderId="12" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="14" fillId="0" borderId="12" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="14" fillId="0" borderId="11" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="9" fillId="0" borderId="17" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="8" fillId="0" borderId="13" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="9" fillId="0" borderId="20" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="8" fillId="0" borderId="14" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="8" fillId="0" borderId="11" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="15" fillId="2" borderId="0" numFmtId="0" xfId="6" applyFont="1" applyFill="1"/>
-    <xf fontId="0" fillId="0" borderId="15" numFmtId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="15" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="13" fillId="0" borderId="15" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="13" fillId="0" borderId="16" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="8" fillId="0" borderId="17" numFmtId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="8" fillId="0" borderId="18" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="8" fillId="0" borderId="19" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="8" fillId="0" borderId="12" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="13" fillId="0" borderId="12" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="8" fillId="0" borderId="17" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="8" fillId="0" borderId="20" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="8" fillId="0" borderId="21" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="9" fillId="0" borderId="21" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="14">
+  <cellStyles count="15">
     <cellStyle name="Style 1" xfId="0" builtinId="0"/>
     <cellStyle name="Style 2" xfId="1" builtinId="3"/>
     <cellStyle name="Style 3" xfId="2" builtinId="6"/>
@@ -743,6 +751,7 @@
     <cellStyle name="60% - Accent1" xfId="11" builtinId="32"/>
     <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
     <cellStyle name="Neutral" xfId="13" builtinId="28"/>
+    <cellStyle name="Bad" xfId="14" builtinId="27"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -8835,7 +8844,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView showGridLines="1" showRowColHeaders="1" workbookViewId="0" zoomScale="100">
+    <sheetView showGridLines="0" showRowColHeaders="1" workbookViewId="0" zoomScale="100">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -8932,7 +8941,7 @@
       <c r="C4" s="6">
         <v>0.089999999999999997</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="22">
         <v>1.1599999999999999</v>
       </c>
       <c r="E4" s="6">
@@ -8964,7 +8973,7 @@
       </c>
     </row>
     <row r="5" ht="19.5" customHeight="1">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="23" t="s">
         <v>55</v>
       </c>
       <c r="B5">
@@ -8997,7 +9006,7 @@
       <c r="K5">
         <v>0.11524232500000001</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="24">
         <v>0.14632896100000001</v>
       </c>
       <c r="M5">
@@ -9005,7 +9014,7 @@
       </c>
     </row>
     <row r="6" ht="19.5" customHeight="1">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="25" t="s">
         <v>56</v>
       </c>
       <c r="B6">
@@ -9046,7 +9055,7 @@
       </c>
     </row>
     <row r="7" ht="19.5" customHeight="1">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="25" t="s">
         <v>57</v>
       </c>
       <c r="B7">
@@ -9055,7 +9064,7 @@
       <c r="C7">
         <v>0.60010004400000005</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="24">
         <v>0.64101926600000003</v>
       </c>
       <c r="E7">
@@ -9087,7 +9096,7 @@
       </c>
     </row>
     <row r="8" ht="19.5" customHeight="1">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="25" t="s">
         <v>58</v>
       </c>
       <c r="B8">
@@ -9120,7 +9129,7 @@
       <c r="K8">
         <v>0.15525059799999999</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="22">
         <v>0.29455088600000001</v>
       </c>
       <c r="M8">
@@ -9128,7 +9137,7 @@
       </c>
     </row>
     <row r="9" ht="19.5" customHeight="1">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="25" t="s">
         <v>59</v>
       </c>
       <c r="B9">
@@ -9169,7 +9178,7 @@
       </c>
     </row>
     <row r="10" ht="19.5" customHeight="1">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="25" t="s">
         <v>60</v>
       </c>
       <c r="B10">
@@ -9190,7 +9199,7 @@
       <c r="G10">
         <v>0.32069843199999998</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="22">
         <v>0.61020401899999999</v>
       </c>
       <c r="I10">
@@ -9210,7 +9219,7 @@
       </c>
     </row>
     <row r="11" ht="19.5" customHeight="1">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="25" t="s">
         <v>61</v>
       </c>
       <c r="B11">
@@ -9251,7 +9260,7 @@
       </c>
     </row>
     <row r="12" ht="19.5" customHeight="1">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="25" t="s">
         <v>62</v>
       </c>
       <c r="B12">
@@ -9260,7 +9269,7 @@
       <c r="C12" s="6">
         <v>0.59048100820771687</v>
       </c>
-      <c r="D12" s="24">
+      <c r="D12" s="6">
         <v>0.64352444392715802</v>
       </c>
       <c r="E12" s="6">
@@ -9272,7 +9281,7 @@
       <c r="G12" s="6">
         <v>0.19352668288310054</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="24">
         <v>0.23190427931161395</v>
       </c>
       <c r="I12" s="6">
@@ -9294,44 +9303,44 @@
     <row r="13" ht="19.5" customHeight="1"/>
     <row r="14" ht="19.5" customHeight="1">
       <c r="A14" s="6"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="27" t="s">
+      <c r="B14" s="26"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="26"/>
-      <c r="M14" s="26"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="27"/>
     </row>
     <row r="15" ht="19.5" customHeight="1">
-      <c r="A15" s="28"/>
-      <c r="B15" s="29" t="s">
+      <c r="A15" s="29"/>
+      <c r="B15" s="30" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="31" t="s">
+      <c r="E15" s="31"/>
+      <c r="F15" s="32" t="s">
         <v>9</v>
       </c>
       <c r="G15" s="16"/>
       <c r="H15" s="16"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="31" t="s">
+      <c r="I15" s="31"/>
+      <c r="J15" s="32" t="s">
         <v>10</v>
       </c>
       <c r="K15" s="16"/>
       <c r="L15" s="16"/>
-      <c r="M15" s="32"/>
+      <c r="M15" s="33"/>
     </row>
     <row r="16" ht="19.5" customHeight="1">
-      <c r="A16" s="33"/>
+      <c r="A16" s="34"/>
       <c r="B16" s="18" t="s">
         <v>50</v>
       </c>
@@ -9341,7 +9350,7 @@
       <c r="D16" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="E16" s="34" t="s">
+      <c r="E16" s="35" t="s">
         <v>53</v>
       </c>
       <c r="F16" s="20" t="s">
@@ -9353,7 +9362,7 @@
       <c r="H16" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="I16" s="34" t="s">
+      <c r="I16" s="35" t="s">
         <v>53</v>
       </c>
       <c r="J16" s="20" t="s">
@@ -9370,7 +9379,7 @@
       </c>
     </row>
     <row r="17" ht="19.5" customHeight="1">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="36" t="s">
         <v>54</v>
       </c>
       <c r="B17" s="12">
@@ -9379,7 +9388,7 @@
       <c r="C17">
         <v>0.089999999999999997</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="22">
         <v>1.03</v>
       </c>
       <c r="E17">
@@ -9411,7 +9420,7 @@
       </c>
     </row>
     <row r="18" ht="19.5" customHeight="1">
-      <c r="A18" s="36" t="s">
+      <c r="A18" s="37" t="s">
         <v>55</v>
       </c>
       <c r="B18">
@@ -9420,7 +9429,7 @@
       <c r="C18">
         <v>0.348900604</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="24">
         <v>0.42071336999999998</v>
       </c>
       <c r="E18">
@@ -9452,7 +9461,7 @@
       </c>
     </row>
     <row r="19" ht="19.5" customHeight="1">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="25" t="s">
         <v>56</v>
       </c>
       <c r="B19">
@@ -9473,7 +9482,7 @@
       <c r="G19">
         <v>0.68420450099999996</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="22">
         <v>0.75608234500000004</v>
       </c>
       <c r="I19">
@@ -9485,7 +9494,7 @@
       <c r="K19">
         <v>0.68420450099999996</v>
       </c>
-      <c r="L19">
+      <c r="L19" s="22">
         <v>0.75608234500000004</v>
       </c>
       <c r="M19">
@@ -9493,7 +9502,7 @@
       </c>
     </row>
     <row r="20" ht="19.5" customHeight="1">
-      <c r="A20" s="23" t="s">
+      <c r="A20" s="25" t="s">
         <v>57</v>
       </c>
       <c r="B20">
@@ -9534,7 +9543,7 @@
       </c>
     </row>
     <row r="21" ht="19.5" customHeight="1">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="25" t="s">
         <v>58</v>
       </c>
       <c r="B21">
@@ -9575,7 +9584,7 @@
       </c>
     </row>
     <row r="22" ht="19.5" customHeight="1">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="25" t="s">
         <v>59</v>
       </c>
       <c r="B22">
@@ -9616,7 +9625,7 @@
       </c>
     </row>
     <row r="23" ht="19.5" customHeight="1">
-      <c r="A23" s="23" t="s">
+      <c r="A23" s="25" t="s">
         <v>60</v>
       </c>
       <c r="B23">
@@ -9657,7 +9666,7 @@
       </c>
     </row>
     <row r="24" ht="19.5" customHeight="1">
-      <c r="A24" s="23" t="s">
+      <c r="A24" s="25" t="s">
         <v>61</v>
       </c>
       <c r="B24">
@@ -9678,7 +9687,7 @@
       <c r="G24">
         <v>0.22276464700000001</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="24">
         <v>0.25337648800000001</v>
       </c>
       <c r="I24">
@@ -9698,7 +9707,7 @@
       </c>
     </row>
     <row r="25" ht="19.5" customHeight="1">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="25" t="s">
         <v>62</v>
       </c>
       <c r="B25">
@@ -9731,7 +9740,7 @@
       <c r="K25" s="6">
         <v>0.12794817952009666</v>
       </c>
-      <c r="L25" s="6">
+      <c r="L25" s="24">
         <v>0.19932011084591655</v>
       </c>
       <c r="M25" s="6">

</xml_diff>

<commit_message>
feat: primer draft de la practica completado
</commit_message>
<xml_diff>
--- a/analisis/Segunda Memoria/Tablas_PAR_2020-21.xlsx
+++ b/analisis/Segunda Memoria/Tablas_PAR_2020-21.xlsx
@@ -7,14 +7,15 @@
   </bookViews>
   <sheets>
     <sheet name="Resultados globales" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Resultados Resumidos" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Desviaciones Típicas Fitness" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Resultados Resumidos" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t xml:space="preserve">Tabla: Información por Problema</t>
   </si>
@@ -163,6 +164,36 @@
     <t>MemeticElitist</t>
   </si>
   <si>
+    <t>Algoritmo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desviacion tipica Fitness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Busqueda local</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genético Generacional Uniforme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genético Generacional Segmento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genético Estacionario Uniforme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genético Estacionario Segmento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memético - Todos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memético - Aleatorio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memético - Elitista</t>
+  </si>
+  <si>
     <t xml:space="preserve">Resultados globales en el PAR con 10% de restricciones</t>
   </si>
   <si>
@@ -194,15 +225,6 @@
   </si>
   <si>
     <t xml:space="preserve">Genético Estacionario - Cruce Segmento</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Memético - Todos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Memético - Aleatorio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Memético - Elitista</t>
   </si>
   <si>
     <t xml:space="preserve">Resultados globales en el PAR con 20% de restricciones</t>
@@ -308,7 +330,7 @@
       <sz val="12.000000"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -356,6 +378,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
   </fills>
@@ -631,7 +659,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="16">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -647,8 +675,9 @@
     <xf fontId="2" fillId="7" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="7" fillId="8" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="8" fillId="9" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
+    <xf fontId="2" fillId="10" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="9" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -667,6 +696,7 @@
     <xf fontId="3" fillId="4" borderId="1" numFmtId="0" xfId="8" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="7" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="12" fillId="6" borderId="0" numFmtId="0" xfId="11" applyFont="1" applyFill="1"/>
+    <xf fontId="2" fillId="10" borderId="0" numFmtId="0" xfId="15" applyFont="1" applyFill="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
     <xf fontId="14" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -736,7 +766,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="16">
     <cellStyle name="Style 1" xfId="0" builtinId="0"/>
     <cellStyle name="Style 2" xfId="1" builtinId="3"/>
     <cellStyle name="Style 3" xfId="2" builtinId="6"/>
@@ -752,6 +782,7 @@
     <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
     <cellStyle name="Neutral" xfId="13" builtinId="28"/>
     <cellStyle name="Bad" xfId="14" builtinId="27"/>
+    <cellStyle name="20% - Accent1" xfId="15" builtinId="30"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1193,7 +1224,7 @@
     <col bestFit="1" customWidth="1" min="6" max="6" width="18.8515625"/>
     <col bestFit="1" customWidth="1" min="7" max="7" width="22.140625"/>
     <col bestFit="1" customWidth="1" min="8" max="8" width="11.019500000000001"/>
-    <col bestFit="1" customWidth="1" min="9" max="9" width="17.074200000000001"/>
+    <col customWidth="1" min="9" max="9" width="30.7109375"/>
     <col bestFit="1" customWidth="1" min="10" max="257" width="11.019500000000001"/>
   </cols>
   <sheetData>
@@ -8844,6 +8875,107 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="27.00390625"/>
+    <col customWidth="1" min="2" max="2" width="22.00390625"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.25">
+      <c r="A1" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25">
+      <c r="A2" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2">
+        <f>STDEV('Resultados globales'!F11:F50)</f>
+        <v>0.27713417205955149</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25">
+      <c r="A3" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3">
+        <f>STDEV('Resultados globales'!F53:F92)</f>
+        <v>0.21805837819767307</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="A4" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4">
+        <f>STDEV('Resultados globales'!F95:F134)</f>
+        <v>0.20617566942448096</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25">
+      <c r="A5" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5">
+        <f>STDEV('Resultados globales'!F137:F175)</f>
+        <v>0.23490479712178633</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="A6" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6">
+        <f>STDEV('Resultados globales'!F177:F215)</f>
+        <v>0.21622318661510934</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25">
+      <c r="A7" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7">
+        <f>STDEV('Resultados globales'!F217:F255)</f>
+        <v>0.11154742846257674</v>
+      </c>
+    </row>
+    <row r="8" ht="14.25">
+      <c r="A8" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8">
+        <f>STDEV('Resultados globales'!F257:F295)</f>
+        <v>0.23246180923353429</v>
+      </c>
+    </row>
+    <row r="9" ht="14.25">
+      <c r="A9" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9">
+        <f>STDEV('Resultados globales'!F297:F335)</f>
+        <v>0.18051044672741881</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="-1" fitToHeight="1" fitToWidth="1" horizontalDpi="600" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="600"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="1" workbookViewId="0" zoomScale="100">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
@@ -8851,7 +8983,7 @@
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col bestFit="1" customWidth="1" min="1" max="1" width="48.00390625"/>
-    <col bestFit="1" customWidth="1" min="2" max="2" style="12" width="17.140625"/>
+    <col bestFit="1" customWidth="1" min="2" max="2" style="13" width="17.140625"/>
     <col bestFit="1" customWidth="1" min="3" max="3" width="18.00390625"/>
     <col bestFit="1" min="4" max="4" width="7.28125"/>
     <col bestFit="1" customWidth="1" min="5" max="5" width="15.421875"/>
@@ -8866,82 +8998,82 @@
   </cols>
   <sheetData>
     <row r="1" ht="15">
-      <c r="B1" s="12"/>
-      <c r="G1" s="13" t="s">
-        <v>49</v>
+      <c r="B1" s="13"/>
+      <c r="G1" s="14" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="2" ht="12.75">
-      <c r="A2" s="14"/>
-      <c r="B2" s="15" t="s">
+      <c r="A2" s="15"/>
+      <c r="B2" s="16" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="17" t="s">
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
     </row>
     <row r="3" ht="15">
-      <c r="A3" s="14"/>
-      <c r="B3" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>52</v>
+      <c r="A3" s="15"/>
+      <c r="B3" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>62</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="G3" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="H3" s="20" t="s">
-        <v>52</v>
+        <v>63</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>62</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="J3" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="K3" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="L3" s="20" t="s">
-        <v>52</v>
+        <v>63</v>
+      </c>
+      <c r="J3" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="K3" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="L3" s="21" t="s">
+        <v>62</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" ht="15">
-      <c r="A4" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4" s="12">
+      <c r="A4" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="13">
         <v>21.600000000000001</v>
       </c>
       <c r="C4" s="6">
         <v>0.089999999999999997</v>
       </c>
-      <c r="D4" s="22">
+      <c r="D4" s="23">
         <v>1.1599999999999999</v>
       </c>
       <c r="E4" s="6">
@@ -8973,8 +9105,8 @@
       </c>
     </row>
     <row r="5" ht="19.5" customHeight="1">
-      <c r="A5" s="23" t="s">
-        <v>55</v>
+      <c r="A5" s="24" t="s">
+        <v>65</v>
       </c>
       <c r="B5">
         <v>10</v>
@@ -9006,7 +9138,7 @@
       <c r="K5">
         <v>0.11524232500000001</v>
       </c>
-      <c r="L5" s="24">
+      <c r="L5" s="25">
         <v>0.14632896100000001</v>
       </c>
       <c r="M5">
@@ -9014,8 +9146,8 @@
       </c>
     </row>
     <row r="6" ht="19.5" customHeight="1">
-      <c r="A6" s="25" t="s">
-        <v>56</v>
+      <c r="A6" s="26" t="s">
+        <v>66</v>
       </c>
       <c r="B6">
         <v>5.4000000000000004</v>
@@ -9055,8 +9187,8 @@
       </c>
     </row>
     <row r="7" ht="19.5" customHeight="1">
-      <c r="A7" s="25" t="s">
-        <v>57</v>
+      <c r="A7" s="26" t="s">
+        <v>67</v>
       </c>
       <c r="B7">
         <v>5.4000000000000004</v>
@@ -9064,7 +9196,7 @@
       <c r="C7">
         <v>0.60010004400000005</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="25">
         <v>0.64101926600000003</v>
       </c>
       <c r="E7">
@@ -9096,8 +9228,8 @@
       </c>
     </row>
     <row r="8" ht="19.5" customHeight="1">
-      <c r="A8" s="25" t="s">
-        <v>58</v>
+      <c r="A8" s="26" t="s">
+        <v>68</v>
       </c>
       <c r="B8">
         <v>6.25</v>
@@ -9129,7 +9261,7 @@
       <c r="K8">
         <v>0.15525059799999999</v>
       </c>
-      <c r="L8" s="22">
+      <c r="L8" s="23">
         <v>0.29455088600000001</v>
       </c>
       <c r="M8">
@@ -9137,8 +9269,8 @@
       </c>
     </row>
     <row r="9" ht="19.5" customHeight="1">
-      <c r="A9" s="25" t="s">
-        <v>59</v>
+      <c r="A9" s="26" t="s">
+        <v>69</v>
       </c>
       <c r="B9">
         <v>6.4000000000000004</v>
@@ -9178,8 +9310,8 @@
       </c>
     </row>
     <row r="10" ht="19.5" customHeight="1">
-      <c r="A10" s="25" t="s">
-        <v>60</v>
+      <c r="A10" s="26" t="s">
+        <v>56</v>
       </c>
       <c r="B10">
         <v>8.4000000000000004</v>
@@ -9199,7 +9331,7 @@
       <c r="G10">
         <v>0.32069843199999998</v>
       </c>
-      <c r="H10" s="22">
+      <c r="H10" s="23">
         <v>0.61020401899999999</v>
       </c>
       <c r="I10">
@@ -9219,8 +9351,8 @@
       </c>
     </row>
     <row r="11" ht="19.5" customHeight="1">
-      <c r="A11" s="25" t="s">
-        <v>61</v>
+      <c r="A11" s="26" t="s">
+        <v>57</v>
       </c>
       <c r="B11">
         <v>9.5999999999999996</v>
@@ -9260,8 +9392,8 @@
       </c>
     </row>
     <row r="12" ht="19.5" customHeight="1">
-      <c r="A12" s="25" t="s">
-        <v>62</v>
+      <c r="A12" s="26" t="s">
+        <v>58</v>
       </c>
       <c r="B12">
         <v>7</v>
@@ -9281,7 +9413,7 @@
       <c r="G12" s="6">
         <v>0.19352668288310054</v>
       </c>
-      <c r="H12" s="24">
+      <c r="H12" s="25">
         <v>0.23190427931161395</v>
       </c>
       <c r="I12" s="6">
@@ -9303,92 +9435,92 @@
     <row r="13" ht="19.5" customHeight="1"/>
     <row r="14" ht="19.5" customHeight="1">
       <c r="A14" s="6"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="28" t="s">
+      <c r="B14" s="27"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
+    </row>
+    <row r="15" ht="19.5" customHeight="1">
+      <c r="A15" s="30"/>
+      <c r="B15" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="34"/>
+    </row>
+    <row r="16" ht="19.5" customHeight="1">
+      <c r="A16" s="35"/>
+      <c r="B16" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="H14" s="27"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="27"/>
-      <c r="K14" s="27"/>
-      <c r="L14" s="27"/>
-      <c r="M14" s="27"/>
-    </row>
-    <row r="15" ht="19.5" customHeight="1">
-      <c r="A15" s="29"/>
-      <c r="B15" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="31"/>
-      <c r="J15" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="K15" s="16"/>
-      <c r="L15" s="16"/>
-      <c r="M15" s="33"/>
-    </row>
-    <row r="16" ht="19.5" customHeight="1">
-      <c r="A16" s="34"/>
-      <c r="B16" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="D16" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="E16" s="35" t="s">
-        <v>53</v>
-      </c>
-      <c r="F16" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="G16" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="H16" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="I16" s="35" t="s">
-        <v>53</v>
-      </c>
-      <c r="J16" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="K16" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="L16" s="20" t="s">
-        <v>52</v>
+      <c r="F16" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="G16" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="H16" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="I16" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="J16" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="K16" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="L16" s="21" t="s">
+        <v>62</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" ht="19.5" customHeight="1">
-      <c r="A17" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="B17" s="12">
+      <c r="A17" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="13">
         <v>7.4000000000000004</v>
       </c>
       <c r="C17">
         <v>0.089999999999999997</v>
       </c>
-      <c r="D17" s="22">
+      <c r="D17" s="23">
         <v>1.03</v>
       </c>
       <c r="E17">
@@ -9420,8 +9552,8 @@
       </c>
     </row>
     <row r="18" ht="19.5" customHeight="1">
-      <c r="A18" s="37" t="s">
-        <v>55</v>
+      <c r="A18" s="38" t="s">
+        <v>65</v>
       </c>
       <c r="B18">
         <v>69.47142857</v>
@@ -9429,7 +9561,7 @@
       <c r="C18">
         <v>0.348900604</v>
       </c>
-      <c r="D18" s="24">
+      <c r="D18" s="25">
         <v>0.42071336999999998</v>
       </c>
       <c r="E18">
@@ -9461,8 +9593,8 @@
       </c>
     </row>
     <row r="19" ht="19.5" customHeight="1">
-      <c r="A19" s="25" t="s">
-        <v>56</v>
+      <c r="A19" s="26" t="s">
+        <v>66</v>
       </c>
       <c r="B19">
         <v>17.800000000000001</v>
@@ -9482,7 +9614,7 @@
       <c r="G19">
         <v>0.68420450099999996</v>
       </c>
-      <c r="H19" s="22">
+      <c r="H19" s="23">
         <v>0.75608234500000004</v>
       </c>
       <c r="I19">
@@ -9494,7 +9626,7 @@
       <c r="K19">
         <v>0.68420450099999996</v>
       </c>
-      <c r="L19" s="22">
+      <c r="L19" s="23">
         <v>0.75608234500000004</v>
       </c>
       <c r="M19">
@@ -9502,8 +9634,8 @@
       </c>
     </row>
     <row r="20" ht="19.5" customHeight="1">
-      <c r="A20" s="25" t="s">
-        <v>57</v>
+      <c r="A20" s="26" t="s">
+        <v>67</v>
       </c>
       <c r="B20">
         <v>19.399999999999999</v>
@@ -9543,8 +9675,8 @@
       </c>
     </row>
     <row r="21" ht="19.5" customHeight="1">
-      <c r="A21" s="25" t="s">
-        <v>58</v>
+      <c r="A21" s="26" t="s">
+        <v>68</v>
       </c>
       <c r="B21">
         <v>19.600000000000001</v>
@@ -9584,8 +9716,8 @@
       </c>
     </row>
     <row r="22" ht="19.5" customHeight="1">
-      <c r="A22" s="25" t="s">
-        <v>59</v>
+      <c r="A22" s="26" t="s">
+        <v>69</v>
       </c>
       <c r="B22">
         <v>18.800000000000001</v>
@@ -9625,8 +9757,8 @@
       </c>
     </row>
     <row r="23" ht="19.5" customHeight="1">
-      <c r="A23" s="25" t="s">
-        <v>60</v>
+      <c r="A23" s="26" t="s">
+        <v>56</v>
       </c>
       <c r="B23">
         <v>18.800000000000001</v>
@@ -9666,8 +9798,8 @@
       </c>
     </row>
     <row r="24" ht="19.5" customHeight="1">
-      <c r="A24" s="25" t="s">
-        <v>61</v>
+      <c r="A24" s="26" t="s">
+        <v>57</v>
       </c>
       <c r="B24">
         <v>15.199999999999999</v>
@@ -9687,7 +9819,7 @@
       <c r="G24">
         <v>0.22276464700000001</v>
       </c>
-      <c r="H24" s="24">
+      <c r="H24" s="25">
         <v>0.25337648800000001</v>
       </c>
       <c r="I24">
@@ -9707,8 +9839,8 @@
       </c>
     </row>
     <row r="25" ht="19.5" customHeight="1">
-      <c r="A25" s="25" t="s">
-        <v>62</v>
+      <c r="A25" s="26" t="s">
+        <v>58</v>
       </c>
       <c r="B25">
         <v>29</v>
@@ -9740,7 +9872,7 @@
       <c r="K25" s="6">
         <v>0.12794817952009666</v>
       </c>
-      <c r="L25" s="24">
+      <c r="L25" s="25">
         <v>0.19932011084591655</v>
       </c>
       <c r="M25" s="6">

</xml_diff>

<commit_message>
fix: algunas erratas corregidas
</commit_message>
<xml_diff>
--- a/analisis/Segunda Memoria/Tablas_PAR_2020-21.xlsx
+++ b/analisis/Segunda Memoria/Tablas_PAR_2020-21.xlsx
@@ -7,8 +7,8 @@
   </bookViews>
   <sheets>
     <sheet name="Resultados globales" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Desviaciones Típicas Fitness" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Resultados Resumidos" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Resultados Resumidos" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Desviaciones Típicas Fitness" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr/>
 </workbook>
@@ -164,36 +164,6 @@
     <t>MemeticElitist</t>
   </si>
   <si>
-    <t>Algoritmo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Desviacion tipica Fitness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Busqueda local</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Genético Generacional Uniforme</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Genético Generacional Segmento</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Genético Estacionario Uniforme</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Genético Estacionario Segmento</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Memético - Todos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Memético - Aleatorio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Memético - Elitista</t>
-  </si>
-  <si>
     <t xml:space="preserve">Resultados globales en el PAR con 10% de restricciones</t>
   </si>
   <si>
@@ -227,7 +197,37 @@
     <t xml:space="preserve">Genético Estacionario - Cruce Segmento</t>
   </si>
   <si>
+    <t xml:space="preserve">Memético - Todos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memético - Aleatorio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memético - Elitista</t>
+  </si>
+  <si>
     <t xml:space="preserve">Resultados globales en el PAR con 20% de restricciones</t>
+  </si>
+  <si>
+    <t>Algoritmo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desviacion tipica Fitness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Busqueda local</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genético Generacional Uniforme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genético Generacional Segmento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genético Estacionario Uniforme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genético Estacionario Segmento</t>
   </si>
 </sst>
 </file>
@@ -696,7 +696,6 @@
     <xf fontId="3" fillId="4" borderId="1" numFmtId="0" xfId="8" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="7" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="12" fillId="6" borderId="0" numFmtId="0" xfId="11" applyFont="1" applyFill="1"/>
-    <xf fontId="2" fillId="10" borderId="0" numFmtId="0" xfId="15" applyFont="1" applyFill="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
     <xf fontId="14" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -765,6 +764,7 @@
     <xf fontId="9" fillId="0" borderId="21" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf fontId="2" fillId="10" borderId="0" numFmtId="0" xfId="15" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="Style 1" xfId="0" builtinId="0"/>
@@ -8875,107 +8875,6 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100">
-      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
-  <cols>
-    <col customWidth="1" min="1" max="1" width="27.00390625"/>
-    <col customWidth="1" min="2" max="2" width="22.00390625"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="14.25">
-      <c r="A1" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" ht="14.25">
-      <c r="A2" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2">
-        <f>STDEV('Resultados globales'!F11:F50)</f>
-        <v>0.27713417205955149</v>
-      </c>
-    </row>
-    <row r="3" ht="14.25">
-      <c r="A3" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="B3">
-        <f>STDEV('Resultados globales'!F53:F92)</f>
-        <v>0.21805837819767307</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25">
-      <c r="A4" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4">
-        <f>STDEV('Resultados globales'!F95:F134)</f>
-        <v>0.20617566942448096</v>
-      </c>
-    </row>
-    <row r="5" ht="14.25">
-      <c r="A5" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5">
-        <f>STDEV('Resultados globales'!F137:F175)</f>
-        <v>0.23490479712178633</v>
-      </c>
-    </row>
-    <row r="6" ht="14.25">
-      <c r="A6" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6">
-        <f>STDEV('Resultados globales'!F177:F215)</f>
-        <v>0.21622318661510934</v>
-      </c>
-    </row>
-    <row r="7" ht="14.25">
-      <c r="A7" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="B7">
-        <f>STDEV('Resultados globales'!F217:F255)</f>
-        <v>0.11154742846257674</v>
-      </c>
-    </row>
-    <row r="8" ht="14.25">
-      <c r="A8" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B8">
-        <f>STDEV('Resultados globales'!F257:F295)</f>
-        <v>0.23246180923353429</v>
-      </c>
-    </row>
-    <row r="9" ht="14.25">
-      <c r="A9" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="B9">
-        <f>STDEV('Resultados globales'!F297:F335)</f>
-        <v>0.18051044672741881</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="-1" fitToHeight="1" fitToWidth="1" horizontalDpi="600" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="600"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
-  <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="1" workbookViewId="0" zoomScale="100">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
@@ -8983,7 +8882,7 @@
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col bestFit="1" customWidth="1" min="1" max="1" width="48.00390625"/>
-    <col bestFit="1" customWidth="1" min="2" max="2" style="13" width="17.140625"/>
+    <col bestFit="1" customWidth="1" min="2" max="2" style="12" width="17.140625"/>
     <col bestFit="1" customWidth="1" min="3" max="3" width="18.00390625"/>
     <col bestFit="1" min="4" max="4" width="7.28125"/>
     <col bestFit="1" customWidth="1" min="5" max="5" width="15.421875"/>
@@ -8998,82 +8897,82 @@
   </cols>
   <sheetData>
     <row r="1" ht="15">
-      <c r="B1" s="13"/>
-      <c r="G1" s="14" t="s">
-        <v>59</v>
+      <c r="B1" s="12"/>
+      <c r="G1" s="13" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="2" ht="12.75">
-      <c r="A2" s="15"/>
-      <c r="B2" s="16" t="s">
+      <c r="A2" s="14"/>
+      <c r="B2" s="15" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="18" t="s">
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
     </row>
     <row r="3" ht="15">
-      <c r="A3" s="15"/>
-      <c r="B3" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>62</v>
+      <c r="A3" s="14"/>
+      <c r="B3" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>52</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F3" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="G3" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="H3" s="21" t="s">
-        <v>62</v>
+        <v>53</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>52</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="J3" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="K3" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="L3" s="21" t="s">
-        <v>62</v>
+        <v>53</v>
+      </c>
+      <c r="J3" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="L3" s="20" t="s">
+        <v>52</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" ht="15">
-      <c r="A4" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" s="13">
+      <c r="A4" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="12">
         <v>21.600000000000001</v>
       </c>
       <c r="C4" s="6">
         <v>0.089999999999999997</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="22">
         <v>1.1599999999999999</v>
       </c>
       <c r="E4" s="6">
@@ -9105,8 +9004,8 @@
       </c>
     </row>
     <row r="5" ht="19.5" customHeight="1">
-      <c r="A5" s="24" t="s">
-        <v>65</v>
+      <c r="A5" s="23" t="s">
+        <v>55</v>
       </c>
       <c r="B5">
         <v>10</v>
@@ -9138,7 +9037,7 @@
       <c r="K5">
         <v>0.11524232500000001</v>
       </c>
-      <c r="L5" s="25">
+      <c r="L5" s="24">
         <v>0.14632896100000001</v>
       </c>
       <c r="M5">
@@ -9146,8 +9045,8 @@
       </c>
     </row>
     <row r="6" ht="19.5" customHeight="1">
-      <c r="A6" s="26" t="s">
-        <v>66</v>
+      <c r="A6" s="25" t="s">
+        <v>56</v>
       </c>
       <c r="B6">
         <v>5.4000000000000004</v>
@@ -9187,8 +9086,8 @@
       </c>
     </row>
     <row r="7" ht="19.5" customHeight="1">
-      <c r="A7" s="26" t="s">
-        <v>67</v>
+      <c r="A7" s="25" t="s">
+        <v>57</v>
       </c>
       <c r="B7">
         <v>5.4000000000000004</v>
@@ -9196,7 +9095,7 @@
       <c r="C7">
         <v>0.60010004400000005</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="24">
         <v>0.64101926600000003</v>
       </c>
       <c r="E7">
@@ -9228,8 +9127,8 @@
       </c>
     </row>
     <row r="8" ht="19.5" customHeight="1">
-      <c r="A8" s="26" t="s">
-        <v>68</v>
+      <c r="A8" s="25" t="s">
+        <v>58</v>
       </c>
       <c r="B8">
         <v>6.25</v>
@@ -9261,7 +9160,7 @@
       <c r="K8">
         <v>0.15525059799999999</v>
       </c>
-      <c r="L8" s="23">
+      <c r="L8" s="22">
         <v>0.29455088600000001</v>
       </c>
       <c r="M8">
@@ -9269,8 +9168,8 @@
       </c>
     </row>
     <row r="9" ht="19.5" customHeight="1">
-      <c r="A9" s="26" t="s">
-        <v>69</v>
+      <c r="A9" s="25" t="s">
+        <v>59</v>
       </c>
       <c r="B9">
         <v>6.4000000000000004</v>
@@ -9310,8 +9209,8 @@
       </c>
     </row>
     <row r="10" ht="19.5" customHeight="1">
-      <c r="A10" s="26" t="s">
-        <v>56</v>
+      <c r="A10" s="25" t="s">
+        <v>60</v>
       </c>
       <c r="B10">
         <v>8.4000000000000004</v>
@@ -9331,7 +9230,7 @@
       <c r="G10">
         <v>0.32069843199999998</v>
       </c>
-      <c r="H10" s="23">
+      <c r="H10" s="22">
         <v>0.61020401899999999</v>
       </c>
       <c r="I10">
@@ -9351,8 +9250,8 @@
       </c>
     </row>
     <row r="11" ht="19.5" customHeight="1">
-      <c r="A11" s="26" t="s">
-        <v>57</v>
+      <c r="A11" s="25" t="s">
+        <v>61</v>
       </c>
       <c r="B11">
         <v>9.5999999999999996</v>
@@ -9392,8 +9291,8 @@
       </c>
     </row>
     <row r="12" ht="19.5" customHeight="1">
-      <c r="A12" s="26" t="s">
-        <v>58</v>
+      <c r="A12" s="25" t="s">
+        <v>62</v>
       </c>
       <c r="B12">
         <v>7</v>
@@ -9413,7 +9312,7 @@
       <c r="G12" s="6">
         <v>0.19352668288310054</v>
       </c>
-      <c r="H12" s="25">
+      <c r="H12" s="24">
         <v>0.23190427931161395</v>
       </c>
       <c r="I12" s="6">
@@ -9435,92 +9334,92 @@
     <row r="13" ht="19.5" customHeight="1"/>
     <row r="14" ht="19.5" customHeight="1">
       <c r="A14" s="6"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="28"/>
-      <c r="L14" s="28"/>
-      <c r="M14" s="28"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="27"/>
     </row>
     <row r="15" ht="19.5" customHeight="1">
-      <c r="A15" s="30"/>
-      <c r="B15" s="31" t="s">
+      <c r="A15" s="29"/>
+      <c r="B15" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="33" t="s">
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="32"/>
-      <c r="J15" s="33" t="s">
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="34"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="33"/>
     </row>
     <row r="16" ht="19.5" customHeight="1">
-      <c r="A16" s="35"/>
-      <c r="B16" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="C16" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="D16" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="E16" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="F16" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="G16" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="H16" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="I16" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="J16" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="K16" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="L16" s="21" t="s">
-        <v>62</v>
+      <c r="A16" s="34"/>
+      <c r="B16" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="H16" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="I16" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="J16" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="K16" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="L16" s="20" t="s">
+        <v>52</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" ht="19.5" customHeight="1">
-      <c r="A17" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="B17" s="13">
+      <c r="A17" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="12">
         <v>7.4000000000000004</v>
       </c>
       <c r="C17">
         <v>0.089999999999999997</v>
       </c>
-      <c r="D17" s="23">
+      <c r="D17" s="22">
         <v>1.03</v>
       </c>
       <c r="E17">
@@ -9552,8 +9451,8 @@
       </c>
     </row>
     <row r="18" ht="19.5" customHeight="1">
-      <c r="A18" s="38" t="s">
-        <v>65</v>
+      <c r="A18" s="37" t="s">
+        <v>55</v>
       </c>
       <c r="B18">
         <v>69.47142857</v>
@@ -9561,7 +9460,7 @@
       <c r="C18">
         <v>0.348900604</v>
       </c>
-      <c r="D18" s="25">
+      <c r="D18" s="24">
         <v>0.42071336999999998</v>
       </c>
       <c r="E18">
@@ -9593,8 +9492,8 @@
       </c>
     </row>
     <row r="19" ht="19.5" customHeight="1">
-      <c r="A19" s="26" t="s">
-        <v>66</v>
+      <c r="A19" s="25" t="s">
+        <v>56</v>
       </c>
       <c r="B19">
         <v>17.800000000000001</v>
@@ -9614,7 +9513,7 @@
       <c r="G19">
         <v>0.68420450099999996</v>
       </c>
-      <c r="H19" s="23">
+      <c r="H19" s="22">
         <v>0.75608234500000004</v>
       </c>
       <c r="I19">
@@ -9626,7 +9525,7 @@
       <c r="K19">
         <v>0.68420450099999996</v>
       </c>
-      <c r="L19" s="23">
+      <c r="L19" s="22">
         <v>0.75608234500000004</v>
       </c>
       <c r="M19">
@@ -9634,8 +9533,8 @@
       </c>
     </row>
     <row r="20" ht="19.5" customHeight="1">
-      <c r="A20" s="26" t="s">
-        <v>67</v>
+      <c r="A20" s="25" t="s">
+        <v>57</v>
       </c>
       <c r="B20">
         <v>19.399999999999999</v>
@@ -9675,8 +9574,8 @@
       </c>
     </row>
     <row r="21" ht="19.5" customHeight="1">
-      <c r="A21" s="26" t="s">
-        <v>68</v>
+      <c r="A21" s="25" t="s">
+        <v>58</v>
       </c>
       <c r="B21">
         <v>19.600000000000001</v>
@@ -9716,8 +9615,8 @@
       </c>
     </row>
     <row r="22" ht="19.5" customHeight="1">
-      <c r="A22" s="26" t="s">
-        <v>69</v>
+      <c r="A22" s="25" t="s">
+        <v>59</v>
       </c>
       <c r="B22">
         <v>18.800000000000001</v>
@@ -9757,8 +9656,8 @@
       </c>
     </row>
     <row r="23" ht="19.5" customHeight="1">
-      <c r="A23" s="26" t="s">
-        <v>56</v>
+      <c r="A23" s="25" t="s">
+        <v>60</v>
       </c>
       <c r="B23">
         <v>18.800000000000001</v>
@@ -9798,8 +9697,8 @@
       </c>
     </row>
     <row r="24" ht="19.5" customHeight="1">
-      <c r="A24" s="26" t="s">
-        <v>57</v>
+      <c r="A24" s="25" t="s">
+        <v>61</v>
       </c>
       <c r="B24">
         <v>15.199999999999999</v>
@@ -9819,7 +9718,7 @@
       <c r="G24">
         <v>0.22276464700000001</v>
       </c>
-      <c r="H24" s="25">
+      <c r="H24" s="24">
         <v>0.25337648800000001</v>
       </c>
       <c r="I24">
@@ -9839,8 +9738,8 @@
       </c>
     </row>
     <row r="25" ht="19.5" customHeight="1">
-      <c r="A25" s="26" t="s">
-        <v>58</v>
+      <c r="A25" s="25" t="s">
+        <v>62</v>
       </c>
       <c r="B25">
         <v>29</v>
@@ -9872,7 +9771,7 @@
       <c r="K25" s="6">
         <v>0.12794817952009666</v>
       </c>
-      <c r="L25" s="25">
+      <c r="L25" s="24">
         <v>0.19932011084591655</v>
       </c>
       <c r="M25" s="6">
@@ -9895,4 +9794,105 @@
   <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="-1" fitToHeight="1" fitToWidth="1" horizontalDpi="600" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="600"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView showGridLines="1" workbookViewId="0" zoomScale="100">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="27.00390625"/>
+    <col customWidth="1" min="2" max="2" width="22.00390625"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.25">
+      <c r="A1" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25">
+      <c r="A2" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2">
+        <f>STDEV('Resultados globales'!F11:F50)</f>
+        <v>0.27713417205955149</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25">
+      <c r="A3" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3">
+        <f>STDEV('Resultados globales'!F53:F92)</f>
+        <v>0.21805837819767307</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="A4" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4">
+        <f>STDEV('Resultados globales'!F95:F134)</f>
+        <v>0.20617566942448096</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25">
+      <c r="A5" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5">
+        <f>STDEV('Resultados globales'!F137:F175)</f>
+        <v>0.23490479712178633</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="A6" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6">
+        <f>STDEV('Resultados globales'!F177:F215)</f>
+        <v>0.21622318661510934</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25">
+      <c r="A7" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7">
+        <f>STDEV('Resultados globales'!F217:F255)</f>
+        <v>0.11154742846257674</v>
+      </c>
+    </row>
+    <row r="8" ht="14.25">
+      <c r="A8" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8">
+        <f>STDEV('Resultados globales'!F257:F295)</f>
+        <v>0.23246180923353429</v>
+      </c>
+    </row>
+    <row r="9" ht="14.25">
+      <c r="A9" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9">
+        <f>STDEV('Resultados globales'!F297:F335)</f>
+        <v>0.18051044672741881</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="-1" fitToHeight="1" fitToWidth="1" horizontalDpi="600" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="600"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>